<commit_message>
adding some laying data
</commit_message>
<xml_diff>
--- a/Nests_masterlist.xlsx
+++ b/Nests_masterlist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justinbenjamin/Desktop/McMaster/Synchrony/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{370FF07C-0209-4842-897A-F2024E2F3C57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16714497-DACD-1242-BA50-983407C51C16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13420" xr2:uid="{0C9768B3-05B5-704F-84A5-5AF5BA71DB46}"/>
   </bookViews>
@@ -5367,8 +5367,8 @@
   <dimension ref="A1:X871"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A435" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H508" sqref="H508"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H206" sqref="H206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5461,7 +5461,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>2008</v>
       </c>
@@ -5623,7 +5623,7 @@
       </c>
       <c r="T5" s="19"/>
     </row>
-    <row r="6" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>2008</v>
       </c>
@@ -7430,7 +7430,7 @@
       </c>
       <c r="T53"/>
     </row>
-    <row r="54" spans="1:20" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:20" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="6">
         <v>2008</v>
       </c>
@@ -7882,7 +7882,7 @@
       <c r="S64" s="18"/>
       <c r="T64" s="19"/>
     </row>
-    <row r="65" spans="1:20" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:20" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="6">
         <v>2008</v>
       </c>
@@ -9932,7 +9932,7 @@
       <c r="S113" s="18"/>
       <c r="T113" s="19"/>
     </row>
-    <row r="114" spans="1:20" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:20" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A114" s="6">
         <v>2010</v>
       </c>
@@ -10402,7 +10402,7 @@
       <c r="S123" s="18"/>
       <c r="T123" s="19"/>
     </row>
-    <row r="124" spans="1:20" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:20" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A124" s="6">
         <v>2010</v>
       </c>
@@ -10586,7 +10586,7 @@
       <c r="S127" s="18"/>
       <c r="T127" s="19"/>
     </row>
-    <row r="128" spans="1:20" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:20" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A128" s="6">
         <v>2010</v>
       </c>
@@ -10927,7 +10927,7 @@
       <c r="S134" s="18"/>
       <c r="T134" s="19"/>
     </row>
-    <row r="135" spans="1:20" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:20" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A135" s="6">
         <v>2010</v>
       </c>
@@ -11139,7 +11139,7 @@
       <c r="S139" s="18"/>
       <c r="T139" s="19"/>
     </row>
-    <row r="140" spans="1:20" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:20" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A140" s="6">
         <v>2010</v>
       </c>
@@ -11180,7 +11180,7 @@
       <c r="S140" s="18"/>
       <c r="T140" s="19"/>
     </row>
-    <row r="141" spans="1:20" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:20" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A141" s="6">
         <v>2010</v>
       </c>
@@ -11481,7 +11481,7 @@
       <c r="S148" s="18"/>
       <c r="T148" s="19"/>
     </row>
-    <row r="149" spans="1:20" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:20" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A149" s="6">
         <v>2013</v>
       </c>
@@ -12222,7 +12222,7 @@
       <c r="S168" s="18"/>
       <c r="T168" s="19"/>
     </row>
-    <row r="169" spans="1:20" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:20" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A169" s="6">
         <v>2014</v>
       </c>
@@ -12398,7 +12398,7 @@
       <c r="S172" s="18"/>
       <c r="T172" s="19"/>
     </row>
-    <row r="173" spans="1:20" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:20" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A173" s="6">
         <v>2014</v>
       </c>
@@ -13367,7 +13367,7 @@
       <c r="S196" s="18"/>
       <c r="T196" s="19"/>
     </row>
-    <row r="197" spans="1:20" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:20" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A197" s="6">
         <v>2014</v>
       </c>
@@ -13487,7 +13487,7 @@
       <c r="S199" s="18"/>
       <c r="T199" s="19"/>
     </row>
-    <row r="200" spans="1:20" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:20" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A200" s="6">
         <v>2014</v>
       </c>
@@ -13640,7 +13640,7 @@
       <c r="S203" s="18"/>
       <c r="T203" s="19"/>
     </row>
-    <row r="204" spans="1:20" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:20" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A204" s="6">
         <v>2014</v>
       </c>
@@ -13685,7 +13685,7 @@
       <c r="S204" s="18"/>
       <c r="T204" s="19"/>
     </row>
-    <row r="205" spans="1:20" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:20" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A205" s="6">
         <v>2014</v>
       </c>
@@ -13730,7 +13730,7 @@
       <c r="S205" s="18"/>
       <c r="T205" s="19"/>
     </row>
-    <row r="206" spans="1:20" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:20" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A206" s="6">
         <v>2014</v>
       </c>
@@ -13778,7 +13778,7 @@
       <c r="S206" s="18"/>
       <c r="T206" s="19"/>
     </row>
-    <row r="207" spans="1:20" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:20" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A207" s="6">
         <v>2014</v>
       </c>
@@ -15673,7 +15673,7 @@
       <c r="S249" s="18"/>
       <c r="T249" s="19"/>
     </row>
-    <row r="250" spans="1:20" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:20" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A250" s="6">
         <v>2015</v>
       </c>
@@ -16111,7 +16111,7 @@
       <c r="S259" s="18"/>
       <c r="T259" s="19"/>
     </row>
-    <row r="260" spans="1:20" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:20" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A260" s="6">
         <v>2015</v>
       </c>
@@ -16162,7 +16162,7 @@
       <c r="S260" s="18"/>
       <c r="T260" s="19"/>
     </row>
-    <row r="261" spans="1:20" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:20" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A261" s="6">
         <v>2015</v>
       </c>
@@ -16332,7 +16332,7 @@
       <c r="S264" s="18"/>
       <c r="T264" s="19"/>
     </row>
-    <row r="265" spans="1:20" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:20" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A265" s="6">
         <v>2015</v>
       </c>
@@ -16475,7 +16475,7 @@
       <c r="S267" s="18"/>
       <c r="T267" s="19"/>
     </row>
-    <row r="268" spans="1:20" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:20" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A268" s="6">
         <v>2015</v>
       </c>
@@ -16563,7 +16563,7 @@
       <c r="S269" s="18"/>
       <c r="T269" s="19"/>
     </row>
-    <row r="270" spans="1:20" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:20" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A270" s="6">
         <v>2015</v>
       </c>
@@ -17313,7 +17313,7 @@
       <c r="S288" s="18"/>
       <c r="T288" s="19"/>
     </row>
-    <row r="289" spans="1:20" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:20" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A289" s="6">
         <v>2015</v>
       </c>
@@ -17445,7 +17445,7 @@
       <c r="S291" s="18"/>
       <c r="T291" s="19"/>
     </row>
-    <row r="292" spans="1:20" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:20" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A292" s="6">
         <v>2015</v>
       </c>
@@ -17663,7 +17663,7 @@
       <c r="S296" s="18"/>
       <c r="T296" s="19"/>
     </row>
-    <row r="297" spans="1:20" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:20" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A297" s="6">
         <v>2015</v>
       </c>
@@ -17987,7 +17987,7 @@
       <c r="S304" s="18"/>
       <c r="T304" s="19"/>
     </row>
-    <row r="305" spans="1:24" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:24" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A305" s="6">
         <v>2015</v>
       </c>
@@ -18703,7 +18703,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="322" spans="1:24" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:24" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A322" s="6">
         <v>2016</v>
       </c>
@@ -18946,7 +18946,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="326" spans="1:24" s="8" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:24" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A326" s="6">
         <v>2016</v>
       </c>
@@ -19055,7 +19055,7 @@
       <c r="W327"/>
       <c r="X327" s="6"/>
     </row>
-    <row r="328" spans="1:24" s="8" customFormat="1" ht="17" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:24" s="8" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A328" s="6">
         <v>2016</v>
       </c>
@@ -19273,7 +19273,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="332" spans="1:24" s="8" customFormat="1" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:24" s="8" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A332" s="6">
         <v>2016</v>
       </c>
@@ -19610,7 +19610,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="338" spans="1:24" s="8" customFormat="1" ht="17" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:24" s="8" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A338" s="6">
         <v>2016</v>
       </c>
@@ -19730,7 +19730,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="340" spans="1:24" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:24" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A340" s="6">
         <v>2016</v>
       </c>
@@ -20070,7 +20070,7 @@
       <c r="S346" s="18"/>
       <c r="T346" s="19"/>
     </row>
-    <row r="347" spans="1:24" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:24" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A347" s="6">
         <v>2016</v>
       </c>
@@ -20433,7 +20433,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="355" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A355" s="6">
         <v>2016</v>
       </c>
@@ -20681,7 +20681,7 @@
       <c r="S360" s="18"/>
       <c r="T360" s="19"/>
     </row>
-    <row r="361" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A361" s="6">
         <v>2016</v>
       </c>
@@ -20906,7 +20906,7 @@
       <c r="S366" s="18"/>
       <c r="T366" s="19"/>
     </row>
-    <row r="367" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A367" s="6">
         <v>2016</v>
       </c>
@@ -20949,7 +20949,7 @@
       <c r="S367" s="18"/>
       <c r="T367" s="19"/>
     </row>
-    <row r="368" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A368" s="6">
         <v>2016</v>
       </c>
@@ -21137,7 +21137,7 @@
       <c r="S371" s="18"/>
       <c r="T371" s="19"/>
     </row>
-    <row r="372" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A372" s="6">
         <v>2016</v>
       </c>
@@ -21251,7 +21251,7 @@
       <c r="S374" s="18"/>
       <c r="T374" s="19"/>
     </row>
-    <row r="375" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A375" s="6">
         <v>2016</v>
       </c>
@@ -21297,7 +21297,7 @@
       <c r="S375" s="18"/>
       <c r="T375" s="19"/>
     </row>
-    <row r="376" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A376" s="6">
         <v>2016</v>
       </c>
@@ -21375,7 +21375,7 @@
       <c r="S377" s="18"/>
       <c r="T377" s="19"/>
     </row>
-    <row r="378" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A378" s="6">
         <v>2016</v>
       </c>
@@ -21784,7 +21784,7 @@
       <c r="S386" s="18"/>
       <c r="T386" s="19"/>
     </row>
-    <row r="387" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A387" s="6">
         <v>2016</v>
       </c>
@@ -21974,7 +21974,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="391" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A391" s="6">
         <v>2016</v>
       </c>
@@ -22686,7 +22686,7 @@
       <c r="T407" s="2"/>
       <c r="U407" s="2"/>
     </row>
-    <row r="408" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A408" s="6">
         <v>2017</v>
       </c>
@@ -22950,7 +22950,7 @@
       <c r="T413" s="2"/>
       <c r="U413" s="2"/>
     </row>
-    <row r="414" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A414" s="6">
         <v>2017</v>
       </c>
@@ -23303,7 +23303,7 @@
       <c r="T421" s="2"/>
       <c r="U421" s="2"/>
     </row>
-    <row r="422" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="422" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A422" s="6">
         <v>2017</v>
       </c>
@@ -23856,7 +23856,7 @@
       <c r="T434" s="2"/>
       <c r="U434" s="2"/>
     </row>
-    <row r="435" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="435" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A435" s="6">
         <v>2018</v>
       </c>
@@ -23903,7 +23903,7 @@
       <c r="T435" s="2"/>
       <c r="U435" s="2"/>
     </row>
-    <row r="436" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="436" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A436" s="6">
         <v>2018</v>
       </c>
@@ -23954,7 +23954,7 @@
       <c r="T436" s="2"/>
       <c r="U436" s="2"/>
     </row>
-    <row r="437" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="437" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A437" s="6">
         <v>2018</v>
       </c>
@@ -24056,7 +24056,7 @@
       <c r="T438" s="2"/>
       <c r="U438" s="2"/>
     </row>
-    <row r="439" spans="1:21" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:21" s="8" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A439" s="6">
         <v>2018</v>
       </c>
@@ -24109,7 +24109,7 @@
       <c r="T439" s="2"/>
       <c r="U439" s="2"/>
     </row>
-    <row r="440" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="440" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A440" s="6">
         <v>2018</v>
       </c>
@@ -24154,7 +24154,7 @@
       <c r="T440" s="2"/>
       <c r="U440" s="2"/>
     </row>
-    <row r="441" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="441" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A441" s="6">
         <v>2018</v>
       </c>
@@ -24203,7 +24203,7 @@
       <c r="T441" s="2"/>
       <c r="U441" s="2"/>
     </row>
-    <row r="442" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="442" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A442" s="6">
         <v>2018</v>
       </c>
@@ -24299,7 +24299,7 @@
       <c r="T443" s="2"/>
       <c r="U443" s="2"/>
     </row>
-    <row r="444" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="444" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A444" s="6">
         <v>2018</v>
       </c>
@@ -24336,7 +24336,7 @@
       <c r="T444" s="2"/>
       <c r="U444" s="2"/>
     </row>
-    <row r="445" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="445" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A445" s="6">
         <v>2018</v>
       </c>
@@ -24385,7 +24385,7 @@
       <c r="T445" s="2"/>
       <c r="U445" s="2"/>
     </row>
-    <row r="446" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="446" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A446" s="6">
         <v>2018</v>
       </c>
@@ -24434,7 +24434,7 @@
       <c r="T446" s="2"/>
       <c r="U446" s="2"/>
     </row>
-    <row r="447" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="447" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A447" s="6">
         <v>2018</v>
       </c>
@@ -24479,7 +24479,7 @@
       <c r="T447" s="2"/>
       <c r="U447" s="2"/>
     </row>
-    <row r="448" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="448" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A448" s="6">
         <v>2018</v>
       </c>
@@ -24526,7 +24526,7 @@
       <c r="T448" s="2"/>
       <c r="U448" s="2"/>
     </row>
-    <row r="449" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="449" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A449" s="6">
         <v>2018</v>
       </c>
@@ -24616,7 +24616,7 @@
       <c r="T450" s="2"/>
       <c r="U450" s="2"/>
     </row>
-    <row r="451" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="451" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A451" s="6">
         <v>2018</v>
       </c>
@@ -24653,7 +24653,7 @@
       <c r="T451" s="2"/>
       <c r="U451" s="2"/>
     </row>
-    <row r="452" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="452" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A452" s="6">
         <v>2018</v>
       </c>
@@ -24702,7 +24702,7 @@
       <c r="T452" s="2"/>
       <c r="U452" s="2"/>
     </row>
-    <row r="453" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="453" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A453" s="6">
         <v>2018</v>
       </c>
@@ -24749,7 +24749,7 @@
       <c r="T453" s="2"/>
       <c r="U453" s="2"/>
     </row>
-    <row r="454" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="454" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A454" s="6">
         <v>2018</v>
       </c>
@@ -24786,7 +24786,7 @@
       <c r="T454" s="2"/>
       <c r="U454" s="2"/>
     </row>
-    <row r="455" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="455" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A455" s="6">
         <v>2018</v>
       </c>
@@ -24833,7 +24833,7 @@
       <c r="T455" s="2"/>
       <c r="U455" s="2"/>
     </row>
-    <row r="456" spans="1:21" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:21" s="8" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A456" s="6">
         <v>2018</v>
       </c>
@@ -24929,7 +24929,7 @@
       <c r="T457" s="2"/>
       <c r="U457" s="2"/>
     </row>
-    <row r="458" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="458" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A458" s="6">
         <v>2018</v>
       </c>
@@ -25013,7 +25013,7 @@
       <c r="T459" s="2"/>
       <c r="U459" s="2"/>
     </row>
-    <row r="460" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="460" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A460" s="6">
         <v>2018</v>
       </c>
@@ -25054,7 +25054,7 @@
       <c r="T460" s="2"/>
       <c r="U460" s="2"/>
     </row>
-    <row r="461" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="461" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A461" s="6">
         <v>2018</v>
       </c>
@@ -25150,7 +25150,7 @@
       <c r="T462" s="2"/>
       <c r="U462" s="2"/>
     </row>
-    <row r="463" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="463" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A463" s="6">
         <v>2018</v>
       </c>
@@ -25199,7 +25199,7 @@
       <c r="T463" s="2"/>
       <c r="U463" s="2"/>
     </row>
-    <row r="464" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="464" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A464" s="6">
         <v>2018</v>
       </c>
@@ -25252,7 +25252,7 @@
       <c r="T464" s="2"/>
       <c r="U464" s="2"/>
     </row>
-    <row r="465" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="465" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A465" s="6">
         <v>2018</v>
       </c>
@@ -25305,7 +25305,7 @@
       <c r="T465" s="2"/>
       <c r="U465" s="2"/>
     </row>
-    <row r="466" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="466" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A466" s="6">
         <v>2018</v>
       </c>
@@ -25354,7 +25354,7 @@
       <c r="T466" s="2"/>
       <c r="U466" s="2"/>
     </row>
-    <row r="467" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="467" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A467" s="6">
         <v>2018</v>
       </c>
@@ -25397,7 +25397,7 @@
       <c r="T467" s="2"/>
       <c r="U467" s="2"/>
     </row>
-    <row r="468" spans="1:21" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:21" s="8" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A468" s="6">
         <v>2018</v>
       </c>
@@ -25591,7 +25591,7 @@
       <c r="T471" s="2"/>
       <c r="U471" s="2"/>
     </row>
-    <row r="472" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="472" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A472" s="6">
         <v>2018</v>
       </c>
@@ -25636,7 +25636,7 @@
       <c r="T472" s="2"/>
       <c r="U472" s="2"/>
     </row>
-    <row r="473" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="473" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A473" s="6">
         <v>2018</v>
       </c>
@@ -25683,7 +25683,7 @@
       <c r="T473" s="2"/>
       <c r="U473" s="2"/>
     </row>
-    <row r="474" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="474" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A474" s="6">
         <v>2018</v>
       </c>
@@ -25726,7 +25726,7 @@
       <c r="T474" s="2"/>
       <c r="U474" s="2"/>
     </row>
-    <row r="475" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="475" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A475" s="6">
         <v>2018</v>
       </c>
@@ -25773,7 +25773,7 @@
       <c r="T475" s="2"/>
       <c r="U475" s="2"/>
     </row>
-    <row r="476" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="476" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A476" s="6">
         <v>2018</v>
       </c>
@@ -25822,7 +25822,7 @@
       <c r="T476" s="2"/>
       <c r="U476" s="2"/>
     </row>
-    <row r="477" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="477" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A477" s="6">
         <v>2018</v>
       </c>
@@ -25869,7 +25869,7 @@
       <c r="T477" s="2"/>
       <c r="U477" s="2"/>
     </row>
-    <row r="478" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="478" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A478" s="6">
         <v>2018</v>
       </c>
@@ -25965,7 +25965,7 @@
       <c r="T479" s="2"/>
       <c r="U479" s="2"/>
     </row>
-    <row r="480" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="480" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A480" s="6">
         <v>2018</v>
       </c>
@@ -26006,7 +26006,7 @@
       <c r="T480" s="2"/>
       <c r="U480" s="2"/>
     </row>
-    <row r="481" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="481" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A481" s="6">
         <v>2018</v>
       </c>
@@ -26047,7 +26047,7 @@
       <c r="T481" s="2"/>
       <c r="U481" s="2"/>
     </row>
-    <row r="482" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="482" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A482" s="6">
         <v>2018</v>
       </c>
@@ -26098,7 +26098,7 @@
       <c r="T482" s="2"/>
       <c r="U482" s="2"/>
     </row>
-    <row r="483" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="483" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A483" s="6">
         <v>2018</v>
       </c>
@@ -26145,7 +26145,7 @@
       <c r="T483" s="2"/>
       <c r="U483" s="2"/>
     </row>
-    <row r="484" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="484" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A484" s="6">
         <v>2018</v>
       </c>
@@ -26243,7 +26243,7 @@
       <c r="T485" s="2"/>
       <c r="U485" s="2"/>
     </row>
-    <row r="486" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="486" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A486" s="6">
         <v>2018</v>
       </c>
@@ -26345,7 +26345,7 @@
       <c r="T487" s="2"/>
       <c r="U487" s="2"/>
     </row>
-    <row r="488" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="488" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A488" s="6">
         <v>2018</v>
       </c>
@@ -26445,7 +26445,7 @@
       <c r="T489" s="2"/>
       <c r="U489" s="2"/>
     </row>
-    <row r="490" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="490" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A490" s="6">
         <v>2018</v>
       </c>
@@ -26496,7 +26496,7 @@
       <c r="T490" s="2"/>
       <c r="U490" s="2"/>
     </row>
-    <row r="491" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="491" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A491" s="6">
         <v>2018</v>
       </c>
@@ -26543,7 +26543,7 @@
       <c r="T491" s="2"/>
       <c r="U491" s="2"/>
     </row>
-    <row r="492" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="492" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A492" s="6">
         <v>2018</v>
       </c>
@@ -26588,7 +26588,7 @@
       <c r="T492" s="2"/>
       <c r="U492" s="2"/>
     </row>
-    <row r="493" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="493" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A493" s="6">
         <v>2018</v>
       </c>
@@ -26684,7 +26684,7 @@
       <c r="T494" s="2"/>
       <c r="U494" s="2"/>
     </row>
-    <row r="495" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="495" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A495" s="6">
         <v>2018</v>
       </c>
@@ -26719,7 +26719,7 @@
       <c r="T495" s="2"/>
       <c r="U495" s="2"/>
     </row>
-    <row r="496" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="496" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A496" s="6">
         <v>2018</v>
       </c>
@@ -26764,7 +26764,7 @@
       <c r="T496" s="2"/>
       <c r="U496" s="2"/>
     </row>
-    <row r="497" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="497" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A497" s="6">
         <v>2018</v>
       </c>
@@ -26803,7 +26803,7 @@
       <c r="T497" s="2"/>
       <c r="U497" s="2"/>
     </row>
-    <row r="498" spans="1:21" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:21" s="8" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A498" s="6">
         <v>2018</v>
       </c>
@@ -26850,7 +26850,7 @@
       <c r="T498" s="2"/>
       <c r="U498" s="2"/>
     </row>
-    <row r="499" spans="1:21" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="499" spans="1:21" s="8" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A499" s="6">
         <v>2018</v>
       </c>
@@ -26895,7 +26895,7 @@
       <c r="T499" s="2"/>
       <c r="U499" s="2"/>
     </row>
-    <row r="500" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="500" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A500" s="6">
         <v>2018</v>
       </c>
@@ -26936,7 +26936,7 @@
       <c r="T500" s="2"/>
       <c r="U500" s="2"/>
     </row>
-    <row r="501" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="501" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A501" s="6">
         <v>2018</v>
       </c>
@@ -26971,7 +26971,7 @@
       <c r="T501" s="2"/>
       <c r="U501" s="2"/>
     </row>
-    <row r="502" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="502" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A502" s="6">
         <v>2018</v>
       </c>
@@ -27010,7 +27010,7 @@
       <c r="T502" s="2"/>
       <c r="U502" s="2"/>
     </row>
-    <row r="503" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="503" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A503" s="6">
         <v>2018</v>
       </c>
@@ -27051,7 +27051,7 @@
       <c r="T503" s="2"/>
       <c r="U503" s="2"/>
     </row>
-    <row r="504" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="504" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A504" s="6">
         <v>2018</v>
       </c>
@@ -27090,7 +27090,7 @@
       <c r="T504" s="2"/>
       <c r="U504" s="2"/>
     </row>
-    <row r="505" spans="1:21" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="505" spans="1:21" s="8" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.25">
       <c r="A505" s="6">
         <v>2018</v>
       </c>
@@ -27133,7 +27133,7 @@
       <c r="T505" s="2"/>
       <c r="U505" s="2"/>
     </row>
-    <row r="506" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="506" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A506" s="6">
         <v>2018</v>
       </c>
@@ -27213,7 +27213,7 @@
       <c r="T507" s="2"/>
       <c r="U507" s="2"/>
     </row>
-    <row r="508" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="508" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A508" s="6">
         <v>2018</v>
       </c>
@@ -27254,7 +27254,7 @@
       <c r="T508" s="2"/>
       <c r="U508" s="2"/>
     </row>
-    <row r="509" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="509" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A509" s="6">
         <v>2018</v>
       </c>
@@ -27299,7 +27299,7 @@
       <c r="T509" s="2"/>
       <c r="U509" s="2"/>
     </row>
-    <row r="510" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="510" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A510" s="6">
         <v>2018</v>
       </c>
@@ -27334,7 +27334,7 @@
       <c r="T510" s="2"/>
       <c r="U510" s="2"/>
     </row>
-    <row r="511" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="511" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A511" s="6">
         <v>2018</v>
       </c>
@@ -27377,7 +27377,7 @@
       <c r="T511" s="2"/>
       <c r="U511" s="2"/>
     </row>
-    <row r="512" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="512" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A512" s="6">
         <v>2018</v>
       </c>
@@ -27416,7 +27416,7 @@
       <c r="T512" s="2"/>
       <c r="U512" s="2"/>
     </row>
-    <row r="513" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="513" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A513" s="6">
         <v>2018</v>
       </c>
@@ -27451,7 +27451,7 @@
       <c r="T513" s="2"/>
       <c r="U513" s="2"/>
     </row>
-    <row r="514" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="514" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A514" s="6">
         <v>2018</v>
       </c>
@@ -27498,7 +27498,7 @@
       <c r="T514" s="2"/>
       <c r="U514" s="2"/>
     </row>
-    <row r="515" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="515" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A515" s="6">
         <v>2018</v>
       </c>
@@ -27537,7 +27537,7 @@
       <c r="T515" s="2"/>
       <c r="U515" s="2"/>
     </row>
-    <row r="516" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="516" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A516" s="6">
         <v>2018</v>
       </c>
@@ -27574,7 +27574,7 @@
       <c r="T516" s="2"/>
       <c r="U516" s="2"/>
     </row>
-    <row r="517" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="517" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A517" s="6">
         <v>2018</v>
       </c>
@@ -27608,7 +27608,7 @@
       <c r="T517" s="2"/>
       <c r="U517" s="2"/>
     </row>
-    <row r="518" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="518" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A518" s="6">
         <v>2018</v>
       </c>
@@ -27649,7 +27649,7 @@
       <c r="T518" s="2"/>
       <c r="U518" s="2"/>
     </row>
-    <row r="519" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="519" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A519" s="6">
         <v>2018</v>
       </c>
@@ -27737,7 +27737,7 @@
       <c r="T520" s="2"/>
       <c r="U520" s="2"/>
     </row>
-    <row r="521" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="521" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A521" s="6">
         <v>2018</v>
       </c>
@@ -27774,7 +27774,7 @@
       <c r="T521" s="2"/>
       <c r="U521" s="2"/>
     </row>
-    <row r="522" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="522" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A522" s="6">
         <v>2018</v>
       </c>
@@ -27808,7 +27808,7 @@
       <c r="T522" s="2"/>
       <c r="U522" s="2"/>
     </row>
-    <row r="523" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="523" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A523" s="6">
         <v>2018</v>
       </c>
@@ -27846,7 +27846,7 @@
       <c r="T523" s="2"/>
       <c r="U523" s="2"/>
     </row>
-    <row r="524" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="524" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A524" s="6">
         <v>2018</v>
       </c>
@@ -27887,7 +27887,7 @@
       <c r="T524" s="2"/>
       <c r="U524" s="2"/>
     </row>
-    <row r="525" spans="1:21" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="525" spans="1:21" s="8" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A525" s="6">
         <v>2018</v>
       </c>
@@ -30485,7 +30485,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="585" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="585" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A585" s="6">
         <v>2022</v>
       </c>
@@ -30985,7 +30985,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="595" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="595" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A595" s="6">
         <v>2022</v>
       </c>
@@ -31392,7 +31392,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="604" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="604" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A604" s="6">
         <v>2022</v>
       </c>
@@ -31502,7 +31502,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="606" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="606" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A606" s="6">
         <v>2022</v>
       </c>
@@ -31834,7 +31834,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="614" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="614" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A614" s="6">
         <v>2022</v>
       </c>
@@ -32002,7 +32002,7 @@
       <c r="T617" s="10"/>
       <c r="U617" s="7"/>
     </row>
-    <row r="618" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="618" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A618" s="6">
         <v>2022</v>
       </c>
@@ -32147,7 +32147,7 @@
       <c r="T620" s="10"/>
       <c r="U620" s="7"/>
     </row>
-    <row r="621" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="621" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A621" s="6">
         <v>2022</v>
       </c>
@@ -32196,7 +32196,7 @@
       <c r="T621" s="10"/>
       <c r="U621" s="7"/>
     </row>
-    <row r="622" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="622" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A622" s="6">
         <v>2022</v>
       </c>
@@ -32349,7 +32349,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="625" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="625" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A625" s="6">
         <v>2022</v>
       </c>
@@ -32404,7 +32404,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="626" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="626" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A626" s="6">
         <v>2022</v>
       </c>
@@ -32459,7 +32459,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="627" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="627" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A627" s="6">
         <v>2022</v>
       </c>
@@ -32553,7 +32553,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="629" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="629" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A629" s="6">
         <v>2022</v>
       </c>
@@ -32657,7 +32657,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="631" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="631" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A631" s="6">
         <v>2022</v>
       </c>
@@ -32855,7 +32855,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="635" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="635" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A635" s="6">
         <v>2022</v>
       </c>
@@ -33010,7 +33010,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="638" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="638" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A638" s="6">
         <v>2022</v>
       </c>
@@ -33065,7 +33065,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="639" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="639" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A639" s="6">
         <v>2022</v>
       </c>
@@ -33222,7 +33222,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="642" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="642" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A642" s="6">
         <v>2022</v>
       </c>
@@ -33592,7 +33592,7 @@
       <c r="T649" s="10"/>
       <c r="U649" s="7"/>
     </row>
-    <row r="650" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="650" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A650" s="6">
         <v>2022</v>
       </c>
@@ -33764,7 +33764,7 @@
       <c r="T653" s="10"/>
       <c r="U653" s="7"/>
     </row>
-    <row r="654" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="654" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A654" s="6">
         <v>2022</v>
       </c>
@@ -33889,7 +33889,7 @@
       <c r="T656" s="10"/>
       <c r="U656" s="7"/>
     </row>
-    <row r="657" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="657" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A657" s="6">
         <v>2022</v>
       </c>
@@ -33977,7 +33977,7 @@
       <c r="T658" s="10"/>
       <c r="U658" s="7"/>
     </row>
-    <row r="659" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="659" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A659" s="6">
         <v>2022</v>
       </c>
@@ -34067,7 +34067,7 @@
       <c r="T660" s="10"/>
       <c r="U660" s="7"/>
     </row>
-    <row r="661" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="661" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A661" s="6">
         <v>2022</v>
       </c>
@@ -34157,7 +34157,7 @@
       <c r="T662" s="10"/>
       <c r="U662" s="7"/>
     </row>
-    <row r="663" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="663" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A663" s="6">
         <v>2022</v>
       </c>
@@ -34202,7 +34202,7 @@
       <c r="T663" s="10"/>
       <c r="U663" s="7"/>
     </row>
-    <row r="664" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="664" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A664" s="6">
         <v>2022</v>
       </c>
@@ -34247,7 +34247,7 @@
       <c r="T664" s="10"/>
       <c r="U664" s="7"/>
     </row>
-    <row r="665" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="665" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A665" s="6">
         <v>2022</v>
       </c>
@@ -34296,7 +34296,7 @@
       <c r="T665" s="10"/>
       <c r="U665" s="7"/>
     </row>
-    <row r="666" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="666" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A666" s="6">
         <v>2022</v>
       </c>
@@ -34558,7 +34558,7 @@
       <c r="T671" s="10"/>
       <c r="U671" s="7"/>
     </row>
-    <row r="672" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="672" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A672" s="6">
         <v>2022</v>
       </c>
@@ -34881,7 +34881,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="679" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="679" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A679" s="11">
         <v>2023</v>
       </c>
@@ -35565,7 +35565,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="692" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="692" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A692" s="11">
         <v>2023</v>
       </c>
@@ -35622,7 +35622,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="693" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="693" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A693" s="11">
         <v>2023</v>
       </c>
@@ -35785,7 +35785,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="696" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="696" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A696" s="11">
         <v>2023</v>
       </c>
@@ -35883,7 +35883,7 @@
       <c r="T697" s="10"/>
       <c r="U697" s="7"/>
     </row>
-    <row r="698" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="698" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A698" s="11">
         <v>2023</v>
       </c>
@@ -36124,7 +36124,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="703" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="703" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A703" s="11">
         <v>2023</v>
       </c>
@@ -36357,7 +36357,7 @@
       <c r="T707" s="10"/>
       <c r="U707" s="7"/>
     </row>
-    <row r="708" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="708" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A708" s="11">
         <v>2023</v>
       </c>
@@ -36457,7 +36457,7 @@
       <c r="T709" s="10"/>
       <c r="U709" s="7"/>
     </row>
-    <row r="710" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="710" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A710" s="11">
         <v>2023</v>
       </c>
@@ -36675,7 +36675,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="714" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="714" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A714" s="11">
         <v>2023</v>
       </c>
@@ -36731,7 +36731,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="715" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="715" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A715" s="11">
         <v>2023</v>
       </c>
@@ -36786,7 +36786,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="716" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="716" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A716" s="11">
         <v>2023</v>
       </c>
@@ -37222,7 +37222,7 @@
       <c r="T723" s="10"/>
       <c r="U723" s="7"/>
     </row>
-    <row r="724" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="724" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A724" s="11">
         <v>2023</v>
       </c>
@@ -37329,7 +37329,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="726" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="726" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A726" s="11">
         <v>2023</v>
       </c>
@@ -37474,7 +37474,7 @@
       <c r="T728" s="10"/>
       <c r="U728" s="7"/>
     </row>
-    <row r="729" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="729" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A729" s="11">
         <v>2023</v>
       </c>
@@ -37666,7 +37666,7 @@
       <c r="T732" s="10"/>
       <c r="U732" s="7"/>
     </row>
-    <row r="733" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="733" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A733" s="11">
         <v>2023</v>
       </c>
@@ -38271,7 +38271,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="747" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="747" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A747" s="11">
         <v>2023</v>
       </c>
@@ -38421,7 +38421,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="750" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="750" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A750" s="11">
         <v>2023</v>
       </c>
@@ -38625,7 +38625,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="754" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="754" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A754" s="11">
         <v>2023</v>
       </c>
@@ -38867,7 +38867,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="759" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="759" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A759" s="11">
         <v>2023</v>
       </c>
@@ -38920,7 +38920,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="760" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="760" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A760" s="11">
         <v>2023</v>
       </c>
@@ -40179,7 +40179,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="785" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="785" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A785">
         <v>2024</v>
       </c>
@@ -40638,7 +40638,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="793" spans="1:21" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="793" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A793">
         <v>2024</v>
       </c>
@@ -40918,7 +40918,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="798" spans="1:21" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="798" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A798">
         <v>2024</v>
       </c>
@@ -41139,7 +41139,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="802" spans="1:21" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="802" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A802">
         <v>2024</v>
       </c>
@@ -41198,7 +41198,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="803" spans="1:21" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="803" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A803">
         <v>2024</v>
       </c>
@@ -41483,7 +41483,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="808" spans="1:21" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="808" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A808">
         <v>2024</v>
       </c>
@@ -41822,7 +41822,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="814" spans="1:21" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="814" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A814">
         <v>2024</v>
       </c>
@@ -42643,7 +42643,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="829" spans="1:21" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="829" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A829">
         <v>2024</v>
       </c>
@@ -42800,7 +42800,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="832" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="832" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A832">
         <v>2024</v>
       </c>
@@ -42855,7 +42855,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="833" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="833" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A833">
         <v>2024</v>
       </c>
@@ -43066,7 +43066,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="837" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="837" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A837">
         <v>2024</v>
       </c>
@@ -43326,7 +43326,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="842" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="842" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A842">
         <v>2024</v>
       </c>
@@ -43434,7 +43434,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="844" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="844" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A844">
         <v>2024</v>
       </c>
@@ -43635,7 +43635,7 @@
         <v>1332</v>
       </c>
     </row>
-    <row r="848" spans="1:21" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="848" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A848">
         <v>2024</v>
       </c>
@@ -43946,9 +43946,14 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:U851" xr:uid="{5405B92D-C97B-C34D-B294-5957E6BF21FE}">
-    <filterColumn colId="0">
+    <filterColumn colId="4">
       <filters>
-        <filter val="2018"/>
+        <filter val="FAILED"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="10">
+      <filters>
+        <filter val="0"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>